<commit_message>
- For each invoice number in the Excel file, search for the invoice number. - Extract the invoice details, including Vendor Tax ID, Invoice Item, Total, and Date. - Write the extracted invoice details to an Excel file stored in the project folder.
</commit_message>
<xml_diff>
--- a/Data/Input/VendorID_Input.xlsx
+++ b/Data/Input/VendorID_Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adriano\Meus Arquivos\UiPath\Projetos\UipathAcademy\BasicProjects\ExtractInvoiceDetails\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06981DDF-03FE-4494-AD75-1E0ECFF140AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9752F5-25DC-477F-A042-001BA241605D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,11 +357,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -389,27 +387,82 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>494559</v>
+        <v>839974</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>815068</v>
+        <v>860620</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>845135</v>
+        <v>982436</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>642745</v>
+        <v>694088</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>622888</v>
+        <v>305290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>214298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>710472</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>427043</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>725704</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>333552</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>701177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>948269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>810093</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>706430</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>101584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>407478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>